<commit_message>
feature: improve orphan detection to now display on unique ID in the logs, provide config to ignore list of defined status-es, and ignore records that doesn't have valid unique ID
</commit_message>
<xml_diff>
--- a/tests/sample_input_files/TGT_sample.xlsx
+++ b/tests/sample_input_files/TGT_sample.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29512"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="73" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9178B506-8752-4463-8688-ACB4BE7A7DC8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{66304990-1033-4BB5-9CEE-83A196D7A363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="78">
   <si>
     <t>Record ID</t>
   </si>
@@ -230,6 +230,63 @@
   </si>
   <si>
     <t>Procedure should not be touched.</t>
+  </si>
+  <si>
+    <t>NOT_VALID</t>
+  </si>
+  <si>
+    <t>Record no REC ID</t>
+  </si>
+  <si>
+    <t>Record without REC ID</t>
+  </si>
+  <si>
+    <t>Brad (14583316)</t>
+  </si>
+  <si>
+    <t>Rejected</t>
+  </si>
+  <si>
+    <t>Record without REC ID procedure.</t>
+  </si>
+  <si>
+    <t>Another Record no REC ID</t>
+  </si>
+  <si>
+    <t>Another record that doesn't have REC ID</t>
+  </si>
+  <si>
+    <t>Another record without REC ID procedure.</t>
+  </si>
+  <si>
+    <t>REC-1111</t>
+  </si>
+  <si>
+    <t>A retired record</t>
+  </si>
+  <si>
+    <t>Some retired record description</t>
+  </si>
+  <si>
+    <t>Retired</t>
+  </si>
+  <si>
+    <t>Retired record procedure.</t>
+  </si>
+  <si>
+    <t>REC-0000</t>
+  </si>
+  <si>
+    <t>An orphaned record</t>
+  </si>
+  <si>
+    <t>Orphaned record for sure</t>
+  </si>
+  <si>
+    <t>Orphaned record procedure.</t>
+  </si>
+  <si>
+    <t>REC-0001</t>
   </si>
 </sst>
 </file>
@@ -651,15 +708,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C16" sqref="A15:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.5703125" customWidth="1"/>
     <col min="3" max="3" width="69" customWidth="1"/>
     <col min="4" max="4" width="31.42578125" customWidth="1"/>
@@ -994,6 +1051,196 @@
         <v>3</v>
       </c>
     </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" t="s">
+        <v>72</v>
+      </c>
+      <c r="J12" t="s">
+        <v>72</v>
+      </c>
+      <c r="K12" t="s">
+        <v>72</v>
+      </c>
+      <c r="L12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" t="s">
+        <v>76</v>
+      </c>
+      <c r="J13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" t="s">
+        <v>76</v>
+      </c>
+      <c r="J14" t="s">
+        <v>76</v>
+      </c>
+      <c r="K14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L14">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>